<commit_message>
Update performance dashboard 2025-12-20 01:05
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251220.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251220.xlsx
@@ -604,49 +604,49 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥484,403.00</t>
+          <t>¥1,001,002.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥-515,597.00</t>
+          <t>¥+1,002.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-51.56%</t>
+          <t>+0.10%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+28.71%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-15.813</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>51.61%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-25.7540%</t>
+          <t>0.1002%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>25.8542%</t>
+          <t>0.0000%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -655,7 +655,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>20251219</t>
+          <t>20251218</t>
         </is>
       </c>
     </row>
@@ -1795,49 +1795,49 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥484,403.00</t>
+          <t>¥1,001,002.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥-515,597.00</t>
+          <t>¥+1,002.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-51.56%</t>
+          <t>+0.10%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+28.71%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-15.813</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>51.61%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-25.7540%</t>
+          <t>0.1002%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>25.8542%</t>
+          <t>0.0000%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>20251219</t>
+          <t>20251218</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update performance dashboard 2025-12-20 10:06
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251220.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251220.xlsx
@@ -531,45 +531,45 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥424,262.00</t>
+          <t>¥1,004,526.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥-575,738.00</t>
+          <t>¥+4,526.00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-57.57%</t>
+          <t>+0.45%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+76.65%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>-15.849</v>
+        <v>19.872</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>57.59%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>-28.7738%</t>
+          <t>0.2262%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>28.8193%</t>
+          <t>0.1807%</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -604,26 +604,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥1,001,002.00</t>
+          <t>¥1,004,601.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥+1,002.00</t>
+          <t>¥+4,601.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>+0.10%</t>
+          <t>+0.46%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+28.71%</t>
+          <t>+78.32%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>28.141</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -637,16 +637,16 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.1002%</t>
+          <t>0.2299%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.0000%</t>
+          <t>0.1297%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -655,7 +655,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>20251218</t>
+          <t>20251219</t>
         </is>
       </c>
     </row>
@@ -677,45 +677,45 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>¥407,459.00</t>
+          <t>¥1,003,469.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¥-592,541.00</t>
+          <t>¥+3,469.00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-59.25%</t>
+          <t>+0.35%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+54.70%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>-15.85</v>
+        <v>21.573</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>59.27%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>-29.6135%</t>
+          <t>0.1734%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>29.6593%</t>
+          <t>0.1276%</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -750,45 +750,45 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥552,853.00</t>
+          <t>¥1,001,074.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥-447,147.00</t>
+          <t>¥+1,074.00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-44.71%</t>
+          <t>+0.11%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+14.48%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-15.902</v>
+        <v>9.238</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>44.71%</t>
+          <t>0.04%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>-22.3660%</t>
+          <t>0.0537%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>22.3274%</t>
+          <t>0.0923%</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -1722,45 +1722,45 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥424,262.00</t>
+          <t>¥1,004,526.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥-575,738.00</t>
+          <t>¥+4,526.00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-57.57%</t>
+          <t>+0.45%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+76.65%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>-15.849</v>
+        <v>19.872</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>57.59%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>-28.7738%</t>
+          <t>0.2262%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>28.8193%</t>
+          <t>0.1807%</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1795,26 +1795,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥1,001,002.00</t>
+          <t>¥1,004,601.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥+1,002.00</t>
+          <t>¥+4,601.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>+0.10%</t>
+          <t>+0.46%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+28.71%</t>
+          <t>+78.32%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>28.141</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -1828,16 +1828,16 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.1002%</t>
+          <t>0.2299%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.0000%</t>
+          <t>0.1297%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>20251218</t>
+          <t>20251219</t>
         </is>
       </c>
     </row>
@@ -1868,45 +1868,45 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>¥407,459.00</t>
+          <t>¥1,003,469.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¥-592,541.00</t>
+          <t>¥+3,469.00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-59.25%</t>
+          <t>+0.35%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+54.70%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>-15.85</v>
+        <v>21.573</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>59.27%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>-29.6135%</t>
+          <t>0.1734%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>29.6593%</t>
+          <t>0.1276%</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -1941,45 +1941,45 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥552,853.00</t>
+          <t>¥1,001,074.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥-447,147.00</t>
+          <t>¥+1,074.00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-44.71%</t>
+          <t>+0.11%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+14.48%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-15.902</v>
+        <v>9.238</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>44.71%</t>
+          <t>0.04%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>-22.3660%</t>
+          <t>0.0537%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>22.3274%</t>
+          <t>0.0923%</t>
         </is>
       </c>
       <c r="M5" t="n">

</xml_diff>